<commit_message>
[Modified]: Meeting - 16
</commit_message>
<xml_diff>
--- a/Báo Cáo/Quá trình làm việc/Meeting/Meeting.xlsx
+++ b/Báo Cáo/Quá trình làm việc/Meeting/Meeting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology\Báo Cáo\Quá trình làm việc\Meeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C47E03-65EF-43E0-AA8C-33FD299F1931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD49A01-0EB3-456C-8C9B-AD4C0AA9447F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>Lịch họp</t>
   </si>
@@ -167,13 +167,19 @@
   </si>
   <si>
     <t>04/12/2021</t>
+  </si>
+  <si>
+    <t>10/12/2022</t>
+  </si>
+  <si>
+    <t>15/12/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +337,12 @@
       <b/>
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -415,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -842,23 +854,25 @@
       <left style="medium">
         <color theme="7" tint="0.39994506668294322"/>
       </left>
+      <right style="medium">
+        <color theme="7" tint="0.39994506668294322"/>
+      </right>
+      <top style="medium">
+        <color theme="7" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thick">
+        <color theme="7" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="7" tint="0.39994506668294322"/>
+      </left>
       <right style="thick">
         <color theme="7" tint="-0.249977111117893"/>
       </right>
       <top style="medium">
-        <color theme="7" tint="0.39991454817346722"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="7" tint="0.39994506668294322"/>
-      </left>
-      <right style="medium">
-        <color theme="7" tint="0.39994506668294322"/>
-      </right>
-      <top style="medium">
         <color theme="7" tint="0.39994506668294322"/>
       </top>
       <bottom style="thick">
@@ -870,21 +884,6 @@
       <left style="medium">
         <color theme="7" tint="0.39994506668294322"/>
       </left>
-      <right style="thick">
-        <color theme="7" tint="-0.249977111117893"/>
-      </right>
-      <top style="medium">
-        <color theme="7" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thick">
-        <color theme="7" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="7" tint="0.39994506668294322"/>
-      </left>
       <right style="medium">
         <color theme="7" tint="0.39994506668294322"/>
       </right>
@@ -919,17 +918,6 @@
       <top style="medium">
         <color theme="4" tint="-0.24994659260841701"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="7" tint="0.39994506668294322"/>
-      </left>
-      <right style="thick">
-        <color theme="7" tint="-0.249977111117893"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -977,7 +965,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1114,9 +1102,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1126,7 +1111,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1145,30 +1130,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="37" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="38" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="39" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="39" xfId="7" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="38" xfId="7" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1490,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.88671875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -1543,28 +1525,28 @@
         <v>7</v>
       </c>
       <c r="I2" s="31"/>
-      <c r="J2" s="47" t="s">
+      <c r="J2" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="48" t="s">
+      <c r="M2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="48" t="s">
+      <c r="N2" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="48" t="s">
+      <c r="Q2" s="47" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1591,14 +1573,14 @@
         <v>0.8</v>
       </c>
       <c r="I3" s="32"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="54"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="53"/>
     </row>
     <row r="4" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13">
@@ -1623,14 +1605,14 @@
         <v>0.9</v>
       </c>
       <c r="I4" s="32"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
       <c r="N4" s="34"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="56"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="55"/>
     </row>
     <row r="5" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="12">
@@ -1655,14 +1637,14 @@
         <v>0.85</v>
       </c>
       <c r="I5" s="32"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="56"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="55"/>
     </row>
     <row r="6" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="13">
@@ -1687,14 +1669,14 @@
         <v>0.82</v>
       </c>
       <c r="I6" s="32"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="56"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="55"/>
     </row>
     <row r="7" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12">
@@ -1712,21 +1694,21 @@
       <c r="F7" s="17">
         <v>0.95833333333333337</v>
       </c>
-      <c r="G7" s="58" t="s">
+      <c r="G7" s="57" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="18">
         <v>1</v>
       </c>
       <c r="I7" s="32"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="56"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="55"/>
     </row>
     <row r="8" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
@@ -1735,7 +1717,7 @@
       <c r="C8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="56" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="17">
@@ -1752,13 +1734,13 @@
       </c>
       <c r="I8" s="32"/>
       <c r="J8" s="36"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="56"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="55"/>
     </row>
     <row r="9" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12">
@@ -1783,14 +1765,14 @@
         <v>0.6</v>
       </c>
       <c r="I9" s="32"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="56"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="55"/>
     </row>
     <row r="10" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13">
@@ -1815,14 +1797,14 @@
         <v>0.8</v>
       </c>
       <c r="I10" s="32"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="56"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="55"/>
     </row>
     <row r="11" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="12">
@@ -1847,14 +1829,14 @@
         <v>0.9</v>
       </c>
       <c r="I11" s="32"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="56"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="55"/>
     </row>
     <row r="12" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="13">
@@ -1879,14 +1861,14 @@
         <v>0.92</v>
       </c>
       <c r="I12" s="32"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="56"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="51"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="55"/>
     </row>
     <row r="13" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12">
@@ -1911,14 +1893,14 @@
         <v>1</v>
       </c>
       <c r="I13" s="32"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="56"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="55"/>
     </row>
     <row r="14" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="13">
@@ -1943,13 +1925,13 @@
         <v>0.83</v>
       </c>
       <c r="I14" s="32"/>
-      <c r="J14" s="51"/>
+      <c r="J14" s="50"/>
       <c r="K14" s="35"/>
-      <c r="L14" s="52"/>
+      <c r="L14" s="51"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
       <c r="O14" s="34"/>
-      <c r="P14" s="52"/>
+      <c r="P14" s="51"/>
       <c r="Q14" s="38"/>
     </row>
     <row r="15" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1975,14 +1957,14 @@
         <v>1</v>
       </c>
       <c r="I15" s="32"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="56"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="55"/>
     </row>
     <row r="16" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13">
@@ -2007,14 +1989,14 @@
         <v>0.8</v>
       </c>
       <c r="I16" s="32"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="60"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="58"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="59"/>
     </row>
     <row r="17" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12">
@@ -2023,20 +2005,30 @@
       <c r="C17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="18"/>
+      <c r="D17" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F17" s="17">
+        <v>0.875</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0.6</v>
+      </c>
       <c r="I17" s="32"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="43"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="59"/>
     </row>
     <row r="18" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="13">
@@ -2045,20 +2037,30 @@
       <c r="C18" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="63"/>
+      <c r="D18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="62">
+        <v>0.72</v>
+      </c>
       <c r="I18" s="32"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="64"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="59"/>
     </row>
     <row r="19" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="12">
@@ -2067,11 +2069,11 @@
       <c r="C19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="63"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="62"/>
       <c r="I19" s="32"/>
       <c r="J19" s="39"/>
       <c r="K19" s="40"/>
@@ -2080,7 +2082,7 @@
       <c r="N19" s="41"/>
       <c r="O19" s="41"/>
       <c r="P19" s="42"/>
-      <c r="Q19" s="64"/>
+      <c r="Q19" s="59"/>
     </row>
     <row r="20" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="13">
@@ -2089,11 +2091,11 @@
       <c r="C20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="63"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="62"/>
       <c r="I20" s="32"/>
       <c r="J20" s="39"/>
       <c r="K20" s="40"/>
@@ -2102,7 +2104,7 @@
       <c r="N20" s="41"/>
       <c r="O20" s="41"/>
       <c r="P20" s="42"/>
-      <c r="Q20" s="64"/>
+      <c r="Q20" s="59"/>
     </row>
     <row r="21" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="12">
@@ -2111,11 +2113,11 @@
       <c r="C21" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="63"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="62"/>
       <c r="I21" s="32"/>
       <c r="J21" s="39"/>
       <c r="K21" s="40"/>
@@ -2124,7 +2126,7 @@
       <c r="N21" s="41"/>
       <c r="O21" s="41"/>
       <c r="P21" s="42"/>
-      <c r="Q21" s="64"/>
+      <c r="Q21" s="59"/>
     </row>
     <row r="22" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="13">
@@ -2133,11 +2135,11 @@
       <c r="C22" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="63"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="62"/>
       <c r="I22" s="32"/>
       <c r="J22" s="39"/>
       <c r="K22" s="40"/>
@@ -2146,7 +2148,7 @@
       <c r="N22" s="41"/>
       <c r="O22" s="41"/>
       <c r="P22" s="42"/>
-      <c r="Q22" s="64"/>
+      <c r="Q22" s="59"/>
     </row>
     <row r="23" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="12">
@@ -2155,11 +2157,11 @@
       <c r="C23" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="61"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="63"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="62"/>
       <c r="I23" s="32"/>
       <c r="J23" s="39"/>
       <c r="K23" s="40"/>
@@ -2168,7 +2170,7 @@
       <c r="N23" s="41"/>
       <c r="O23" s="41"/>
       <c r="P23" s="42"/>
-      <c r="Q23" s="64"/>
+      <c r="Q23" s="59"/>
     </row>
     <row r="24" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="13">
@@ -2177,11 +2179,11 @@
       <c r="C24" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="63"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="62"/>
       <c r="I24" s="32"/>
       <c r="J24" s="39"/>
       <c r="K24" s="40"/>
@@ -2190,7 +2192,7 @@
       <c r="N24" s="41"/>
       <c r="O24" s="41"/>
       <c r="P24" s="42"/>
-      <c r="Q24" s="64"/>
+      <c r="Q24" s="59"/>
     </row>
     <row r="25" spans="2:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="12">
@@ -2206,19 +2208,20 @@
       <c r="H25" s="23"/>
       <c r="I25" s="33"/>
       <c r="J25" s="37"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="45"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="44"/>
     </row>
     <row r="26" spans="2:17" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C26" s="14"/>
       <c r="I26" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Tiêu đề của dự án. Nhập tiêu đề mới vào ô này. Tô sáng thời gian trong H2. Chú thích biểu đồ nằm trong J2 đến AI2" sqref="B1:D1" xr:uid="{E5E2E5D2-0AD3-42B7-BE94-EE511D19E99A}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Nhập tỷ lệ phần trăm dự án được hoàn thành vào cột G, bắt đầu với ô G5" sqref="H2:I2" xr:uid="{ED781070-0D85-4665-B52C-D93FBA166C98}"/>

</xml_diff>